<commit_message>
Updated reporting for bordereau
</commit_message>
<xml_diff>
--- a/BillingCentre-DataDriven/src/test/java/Reports/Driver_AQS_SL_S10_Iteration 01.xlsx
+++ b/BillingCentre-DataDriven/src/test/java/Reports/Driver_AQS_SL_S10_Iteration 01.xlsx
@@ -1,36 +1,36 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
   <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="124226" filterPrivacy="1"/>
+  <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView activeTab="15" firstSheet="12" windowHeight="7716" windowWidth="14808" xWindow="240" yWindow="108"/>
+    <workbookView xWindow="240" yWindow="108" windowWidth="14808" windowHeight="7716" firstSheet="12" activeTab="15"/>
   </bookViews>
   <sheets>
-    <sheet name="PHSD1869556" r:id="rId1" sheetId="11"/>
-    <sheet name="PHSD1869558" r:id="rId2" sheetId="13"/>
-    <sheet name="PHSD1869557" r:id="rId3" sheetId="12"/>
-    <sheet name="PHSD1869559" r:id="rId4" sheetId="14"/>
-    <sheet name="PHSD1869560" r:id="rId5" sheetId="15"/>
-    <sheet name="PHSD1869561" r:id="rId6" sheetId="16"/>
-    <sheet name="PHSD1869562" r:id="rId7" sheetId="17"/>
-    <sheet name="Package10_PA_11964169" r:id="rId8" sheetId="25"/>
-    <sheet name="Package10_NY_11964153" r:id="rId9" sheetId="24"/>
-    <sheet name="Package10_CA_11964138" r:id="rId10" sheetId="23"/>
-    <sheet name="Package10_OK_11964127" r:id="rId11" sheetId="22"/>
-    <sheet name="Package10_NJ_11964113" r:id="rId12" sheetId="21"/>
-    <sheet name="Package10_WA_11964099" r:id="rId13" sheetId="20"/>
-    <sheet name="Package10_WV_11964086" r:id="rId14" sheetId="19"/>
-    <sheet name="Package10_MA_11964070" r:id="rId15" sheetId="18"/>
-    <sheet name="Results" r:id="rId16" sheetId="1"/>
-    <sheet name="State_Validations" r:id="rId17" sheetId="10"/>
+    <sheet name="PHSD1869556" sheetId="11" r:id="rId1"/>
+    <sheet name="PHSD1869558" sheetId="13" r:id="rId2"/>
+    <sheet name="PHSD1869557" sheetId="12" r:id="rId3"/>
+    <sheet name="PHSD1869559" sheetId="14" r:id="rId4"/>
+    <sheet name="PHSD1869560" sheetId="15" r:id="rId5"/>
+    <sheet name="PHSD1869561" sheetId="16" r:id="rId6"/>
+    <sheet name="PHSD1869562" sheetId="17" r:id="rId7"/>
+    <sheet name="Package10_PA_11964169" sheetId="25" r:id="rId8"/>
+    <sheet name="Package10_NY_11964153" sheetId="24" r:id="rId9"/>
+    <sheet name="Package10_CA_11964138" sheetId="23" r:id="rId10"/>
+    <sheet name="Package10_OK_11964127" sheetId="22" r:id="rId11"/>
+    <sheet name="Package10_NJ_11964113" sheetId="21" r:id="rId12"/>
+    <sheet name="Package10_WA_11964099" sheetId="20" r:id="rId13"/>
+    <sheet name="Package10_WV_11964086" sheetId="19" r:id="rId14"/>
+    <sheet name="Package10_MA_11964070" sheetId="18" r:id="rId15"/>
+    <sheet name="Results" sheetId="1" r:id="rId16"/>
+    <sheet name="State_Validations" sheetId="10" r:id="rId17"/>
   </sheets>
   <calcPr calcId="125725"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="580" uniqueCount="117">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="538" uniqueCount="106">
   <si>
     <t>Policy Number</t>
   </si>
@@ -348,39 +348,6 @@
   </si>
   <si>
     <t>PR: Pre-Approved Renewal</t>
-  </si>
-  <si>
-    <t>Active</t>
-  </si>
-  <si>
-    <t>Written_Premium</t>
-  </si>
-  <si>
-    <t>Tax</t>
-  </si>
-  <si>
-    <t>$828.00</t>
-  </si>
-  <si>
-    <t>-</t>
-  </si>
-  <si>
-    <t>$2,745.00</t>
-  </si>
-  <si>
-    <t>$962.00</t>
-  </si>
-  <si>
-    <t>$2,064.00</t>
-  </si>
-  <si>
-    <t>$1,597.00</t>
-  </si>
-  <si>
-    <t>$1,000.00</t>
-  </si>
-  <si>
-    <t>$16,769.00</t>
   </si>
 </sst>
 </file>
@@ -416,7 +383,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="21">
+  <fills count="7">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -451,76 +418,6 @@
       <patternFill patternType="solid">
         <fgColor indexed="12"/>
         <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="none">
-        <fgColor indexed="55"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="none">
-        <fgColor indexed="55"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="none">
-        <fgColor indexed="55"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="none">
-        <fgColor indexed="55"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="none">
-        <fgColor indexed="55"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="none">
-        <fgColor indexed="55"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="none">
-        <fgColor indexed="55"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="none">
-        <fgColor indexed="55"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="none">
-        <fgColor indexed="55"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="none">
-        <fgColor indexed="55"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="none">
-        <fgColor indexed="55"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="none">
-        <fgColor indexed="55"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="none">
-        <fgColor indexed="55"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="none">
-        <fgColor indexed="55"/>
       </patternFill>
     </fill>
   </fills>
@@ -562,45 +459,31 @@
     </border>
   </borders>
   <cellStyleXfs count="1">
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="30">
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
-    <xf applyBorder="1" borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
-    <xf applyBorder="1" applyFill="1" applyFont="1" borderId="1" fillId="2" fontId="1" numFmtId="0" xfId="0"/>
-    <xf applyBorder="1" applyFill="1" applyFont="1" borderId="2" fillId="2" fontId="1" numFmtId="0" xfId="0"/>
-    <xf applyFont="1" borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0"/>
-    <xf applyFill="1" applyFont="1" borderId="0" fillId="3" fontId="1" numFmtId="0" xfId="0"/>
-    <xf applyFill="1" applyFont="1" borderId="0" fillId="4" fontId="1" numFmtId="0" xfId="0"/>
-    <xf applyFill="1" applyFont="1" borderId="0" fillId="5" fontId="1" numFmtId="0" xfId="0"/>
-    <xf applyNumberFormat="1" borderId="0" fillId="0" fontId="0" numFmtId="14" xfId="0"/>
-    <xf applyNumberFormat="1" borderId="0" fillId="0" fontId="0" numFmtId="8" xfId="0"/>
-    <xf applyFill="1" borderId="0" fillId="5" fontId="0" numFmtId="0" xfId="0"/>
-    <xf applyFill="1" applyFont="1" borderId="0" fillId="5" fontId="0" numFmtId="0" xfId="0"/>
-    <xf applyFont="1" borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="0"/>
-    <xf applyNumberFormat="1" borderId="0" fillId="0" fontId="0" numFmtId="4" xfId="0"/>
-    <xf applyNumberFormat="1" borderId="0" fillId="0" fontId="0" numFmtId="7" xfId="0"/>
-    <xf applyFill="1" applyFont="1" borderId="0" fillId="6" fontId="1" numFmtId="0" xfId="0"/>
-    <xf applyFill="true" borderId="0" fillId="7" fontId="0" numFmtId="0" xfId="0"/>
-    <xf applyFill="true" borderId="0" fillId="8" fontId="0" numFmtId="0" xfId="0"/>
-    <xf applyFill="true" borderId="0" fillId="9" fontId="0" numFmtId="0" xfId="0"/>
-    <xf applyFill="true" borderId="0" fillId="10" fontId="0" numFmtId="0" xfId="0"/>
-    <xf applyFill="true" borderId="0" fillId="11" fontId="0" numFmtId="0" xfId="0"/>
-    <xf applyFill="true" borderId="0" fillId="12" fontId="0" numFmtId="0" xfId="0"/>
-    <xf applyFill="true" borderId="0" fillId="13" fontId="0" numFmtId="0" xfId="0"/>
-    <xf applyFill="true" borderId="0" fillId="14" fontId="0" numFmtId="0" xfId="0"/>
-    <xf applyFill="true" borderId="0" fillId="15" fontId="0" numFmtId="0" xfId="0"/>
-    <xf applyFill="true" borderId="0" fillId="16" fontId="0" numFmtId="0" xfId="0"/>
-    <xf applyFill="true" borderId="0" fillId="17" fontId="0" numFmtId="0" xfId="0"/>
-    <xf applyFill="true" borderId="0" fillId="18" fontId="0" numFmtId="0" xfId="0"/>
-    <xf applyFill="true" borderId="0" fillId="19" fontId="0" numFmtId="0" xfId="0"/>
-    <xf applyFill="true" borderId="0" fillId="20" fontId="0" numFmtId="0" xfId="0"/>
+  <cellXfs count="16">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="8" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="4" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="7" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle builtinId="0" name="Normal" xfId="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
-  <tableStyles count="0" defaultPivotStyle="PivotStyleLight16" defaultTableStyle="TableStyleMedium9"/>
+  <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
@@ -617,10 +500,10 @@
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
-        <a:sysClr lastClr="000000" val="windowText"/>
+        <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
       <a:lt1>
-        <a:sysClr lastClr="FFFFFF" val="window"/>
+        <a:sysClr val="window" lastClr="FFFFFF"/>
       </a:lt1>
       <a:dk2>
         <a:srgbClr val="1F497D"/>
@@ -655,7 +538,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin panose="020F0302020204030204" typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -690,7 +573,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin panose="020F0502020204030204" typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -778,7 +661,7 @@
         </a:gradFill>
       </a:fillStyleLst>
       <a:lnStyleLst>
-        <a:ln algn="ctr" cap="flat" cmpd="sng" w="9525">
+        <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
           <a:solidFill>
             <a:schemeClr val="phClr">
               <a:shade val="95000"/>
@@ -787,13 +670,13 @@
           </a:solidFill>
           <a:prstDash val="solid"/>
         </a:ln>
-        <a:ln algn="ctr" cap="flat" cmpd="sng" w="25400">
+        <a:ln w="25400" cap="flat" cmpd="sng" algn="ctr">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
           </a:solidFill>
           <a:prstDash val="solid"/>
         </a:ln>
-        <a:ln algn="ctr" cap="flat" cmpd="sng" w="38100">
+        <a:ln w="38100" cap="flat" cmpd="sng" algn="ctr">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
           </a:solidFill>
@@ -803,7 +686,7 @@
       <a:effectStyleLst>
         <a:effectStyle>
           <a:effectLst>
-            <a:outerShdw blurRad="40000" dir="5400000" dist="20000" rotWithShape="0">
+            <a:outerShdw blurRad="40000" dist="20000" dir="5400000" rotWithShape="0">
               <a:srgbClr val="000000">
                 <a:alpha val="38000"/>
               </a:srgbClr>
@@ -812,7 +695,7 @@
         </a:effectStyle>
         <a:effectStyle>
           <a:effectLst>
-            <a:outerShdw blurRad="40000" dir="5400000" dist="23000" rotWithShape="0">
+            <a:outerShdw blurRad="40000" dist="23000" dir="5400000" rotWithShape="0">
               <a:srgbClr val="000000">
                 <a:alpha val="35000"/>
               </a:srgbClr>
@@ -821,7 +704,7 @@
         </a:effectStyle>
         <a:effectStyle>
           <a:effectLst>
-            <a:outerShdw blurRad="40000" dir="5400000" dist="23000" rotWithShape="0">
+            <a:outerShdw blurRad="40000" dist="23000" dir="5400000" rotWithShape="0">
               <a:srgbClr val="000000">
                 <a:alpha val="35000"/>
               </a:srgbClr>
@@ -831,12 +714,12 @@
             <a:camera prst="orthographicFront">
               <a:rot lat="0" lon="0" rev="0"/>
             </a:camera>
-            <a:lightRig dir="t" rig="threePt">
+            <a:lightRig rig="threePt" dir="t">
               <a:rot lat="0" lon="0" rev="1200000"/>
             </a:lightRig>
           </a:scene3d>
           <a:sp3d>
-            <a:bevelT h="25400" w="63500"/>
+            <a:bevelT w="63500" h="25400"/>
           </a:sp3d>
         </a:effectStyle>
       </a:effectStyleLst>
@@ -867,7 +750,7 @@
             </a:gs>
           </a:gsLst>
           <a:path path="circle">
-            <a:fillToRect b="180000" l="50000" r="50000" t="-80000"/>
+            <a:fillToRect l="50000" t="-80000" r="50000" b="180000"/>
           </a:path>
         </a:gradFill>
         <a:gradFill rotWithShape="1">
@@ -886,7 +769,7 @@
             </a:gs>
           </a:gsLst>
           <a:path path="circle">
-            <a:fillToRect b="50000" l="50000" r="50000" t="50000"/>
+            <a:fillToRect l="50000" t="50000" r="50000" b="50000"/>
           </a:path>
         </a:gradFill>
       </a:bgFillStyleLst>
@@ -898,16 +781,12 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:I18"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:H18"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
-  <cols>
-    <col min="5" max="5" bestFit="true" customWidth="true" width="17.2578125" collapsed="true"/>
-    <col min="6" max="6" bestFit="true" customWidth="true" width="8.28125" collapsed="true"/>
-  </cols>
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A1" s="5" t="s">
@@ -922,12 +801,6 @@
       <c r="D1" t="s">
         <v>92</v>
       </c>
-      <c r="E1" s="16" t="s">
-        <v>6</v>
-      </c>
-      <c r="F1" s="17" t="s">
-        <v>106</v>
-      </c>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A2" s="5" t="s">
@@ -936,12 +809,6 @@
       <c r="B2" s="8">
         <v>43362</v>
       </c>
-      <c r="E2" t="s">
-        <v>107</v>
-      </c>
-      <c r="F2" t="s">
-        <v>109</v>
-      </c>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A3" s="5" t="s">
@@ -956,12 +823,6 @@
       <c r="D3" t="s">
         <v>20</v>
       </c>
-      <c r="E3" t="s">
-        <v>108</v>
-      </c>
-      <c r="F3" t="s">
-        <v>110</v>
-      </c>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A4" s="5" t="s">
@@ -1118,14 +979,14 @@
       </c>
     </row>
   </sheetData>
-  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C24"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:B24"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -1283,14 +1144,14 @@
       </c>
     </row>
   </sheetData>
-  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C24"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:B24"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -1448,14 +1309,14 @@
       </c>
     </row>
   </sheetData>
-  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C24"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:B24"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -1613,14 +1474,14 @@
       </c>
     </row>
   </sheetData>
-  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C24"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:B24"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -1778,14 +1639,14 @@
       </c>
     </row>
   </sheetData>
-  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C24"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:B24"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -1943,14 +1804,14 @@
       </c>
     </row>
   </sheetData>
-  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C24"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:B24"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -2108,35 +1969,35 @@
       </c>
     </row>
   </sheetData>
-  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet16.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:N16"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:M16"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0" zoomScaleNormal="100"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" bestFit="true" customWidth="true" width="10.109375" collapsed="true"/>
-    <col min="2" max="2" bestFit="true" customWidth="true" width="14.109375" collapsed="true"/>
-    <col min="3" max="3" bestFit="true" customWidth="true" width="37.0" collapsed="true"/>
-    <col min="4" max="4" bestFit="true" customWidth="true" width="11.6640625" collapsed="true"/>
-    <col min="5" max="5" bestFit="true" customWidth="true" width="5.5546875" collapsed="true"/>
-    <col min="6" max="6" bestFit="true" customWidth="true" width="13.6640625" collapsed="true"/>
-    <col min="7" max="7" bestFit="true" customWidth="true" width="20.44140625" collapsed="true"/>
-    <col min="8" max="8" bestFit="true" customWidth="true" width="22.0" collapsed="true"/>
-    <col min="9" max="9" bestFit="true" customWidth="true" width="9.5546875" collapsed="true"/>
-    <col min="10" max="10" bestFit="true" customWidth="true" width="20.6640625" collapsed="true"/>
-    <col min="11" max="11" bestFit="true" customWidth="true" width="6.44140625" collapsed="true"/>
-    <col min="12" max="12" bestFit="true" customWidth="true" width="21.5546875" collapsed="true"/>
-    <col min="13" max="13" bestFit="true" customWidth="true" width="8.5546875" collapsed="true"/>
+    <col min="1" max="1" width="10.109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="14.109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="37" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="11.6640625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="5.5546875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="13.6640625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="20.44140625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="22" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="9.5546875" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="20.6640625" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="6.44140625" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="21.5546875" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="8.5546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row customHeight="1" ht="15.75" r="1" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A1" s="2" t="s">
         <v>4</v>
       </c>
@@ -2652,28 +2513,28 @@
       </c>
     </row>
   </sheetData>
-  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet17.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G1"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:F1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" bestFit="true" customWidth="true" width="8.109375" collapsed="true"/>
-    <col min="2" max="2" bestFit="true" customWidth="true" width="6.6640625" collapsed="true"/>
-    <col min="3" max="3" bestFit="true" customWidth="true" width="7.88671875" collapsed="true"/>
-    <col min="4" max="4" bestFit="true" customWidth="true" width="4.44140625" collapsed="true"/>
-    <col min="5" max="5" bestFit="true" customWidth="true" width="5.5546875" collapsed="true"/>
-    <col min="6" max="6" bestFit="true" customWidth="true" width="8.5546875" collapsed="true"/>
+    <col min="1" max="1" width="8.109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="6.6640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="7.88671875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="4.44140625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="5.5546875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="8.5546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row customFormat="1" r="1" s="1" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:6" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A1" s="2" t="s">
         <v>4</v>
       </c>
@@ -2694,21 +2555,17 @@
       </c>
     </row>
   </sheetData>
-  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G18"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:D18"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
-  <cols>
-    <col min="5" max="5" bestFit="true" customWidth="true" width="17.2578125" collapsed="true"/>
-    <col min="6" max="6" bestFit="true" customWidth="true" width="8.28125" collapsed="true"/>
-  </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A1" s="5" t="s">
@@ -2723,12 +2580,6 @@
       <c r="D1" t="s">
         <v>92</v>
       </c>
-      <c r="E1" s="20" t="s">
-        <v>6</v>
-      </c>
-      <c r="F1" s="21" t="s">
-        <v>106</v>
-      </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A2" s="5" t="s">
@@ -2737,12 +2588,6 @@
       <c r="B2" s="8">
         <v>43362</v>
       </c>
-      <c r="E2" t="s">
-        <v>107</v>
-      </c>
-      <c r="F2" t="s">
-        <v>112</v>
-      </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A3" s="5" t="s">
@@ -2757,12 +2602,6 @@
       <c r="D3" t="s">
         <v>37</v>
       </c>
-      <c r="E3" t="s">
-        <v>108</v>
-      </c>
-      <c r="F3" t="s">
-        <v>110</v>
-      </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A4" s="5" t="s">
@@ -2873,22 +2712,18 @@
       </c>
     </row>
   </sheetData>
-  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G18"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:D18"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
-  <cols>
-    <col min="5" max="5" bestFit="true" customWidth="true" width="17.2578125" collapsed="true"/>
-    <col min="6" max="6" bestFit="true" customWidth="true" width="9.9453125" collapsed="true"/>
-  </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A1" s="5" t="s">
@@ -2903,12 +2738,6 @@
       <c r="D1" t="s">
         <v>92</v>
       </c>
-      <c r="E1" s="18" t="s">
-        <v>6</v>
-      </c>
-      <c r="F1" s="19" t="s">
-        <v>106</v>
-      </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A2" s="5" t="s">
@@ -2917,12 +2746,6 @@
       <c r="B2" s="8">
         <v>43362</v>
       </c>
-      <c r="E2" t="s">
-        <v>107</v>
-      </c>
-      <c r="F2" t="s">
-        <v>111</v>
-      </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A3" s="5" t="s">
@@ -2937,12 +2760,6 @@
       <c r="D3" t="s">
         <v>31</v>
       </c>
-      <c r="E3" t="s">
-        <v>108</v>
-      </c>
-      <c r="F3" t="s">
-        <v>110</v>
-      </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A4" s="5" t="s">
@@ -3053,22 +2870,18 @@
       </c>
     </row>
   </sheetData>
-  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G18"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:D18"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
-  <cols>
-    <col min="5" max="5" bestFit="true" customWidth="true" width="17.2578125" collapsed="true"/>
-    <col min="6" max="6" bestFit="true" customWidth="true" width="9.9453125" collapsed="true"/>
-  </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A1" s="5" t="s">
@@ -3083,12 +2896,6 @@
       <c r="D1" t="s">
         <v>92</v>
       </c>
-      <c r="E1" s="22" t="s">
-        <v>6</v>
-      </c>
-      <c r="F1" s="23" t="s">
-        <v>106</v>
-      </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A2" s="5" t="s">
@@ -3097,12 +2904,6 @@
       <c r="B2" s="8">
         <v>43362</v>
       </c>
-      <c r="E2" t="s">
-        <v>107</v>
-      </c>
-      <c r="F2" t="s">
-        <v>113</v>
-      </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A3" s="5" t="s">
@@ -3117,12 +2918,6 @@
       <c r="D3" t="s">
         <v>43</v>
       </c>
-      <c r="E3" t="s">
-        <v>108</v>
-      </c>
-      <c r="F3" t="s">
-        <v>110</v>
-      </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A4" s="5" t="s">
@@ -3233,22 +3028,18 @@
       </c>
     </row>
   </sheetData>
-  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G18"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:D18"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
-  <cols>
-    <col min="5" max="5" bestFit="true" customWidth="true" width="17.2578125" collapsed="true"/>
-    <col min="6" max="6" bestFit="true" customWidth="true" width="9.9453125" collapsed="true"/>
-  </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A1" s="5" t="s">
@@ -3263,12 +3054,6 @@
       <c r="D1" t="s">
         <v>92</v>
       </c>
-      <c r="E1" s="24" t="s">
-        <v>6</v>
-      </c>
-      <c r="F1" s="25" t="s">
-        <v>106</v>
-      </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A2" s="5" t="s">
@@ -3277,12 +3062,6 @@
       <c r="B2" s="8">
         <v>43362</v>
       </c>
-      <c r="E2" t="s">
-        <v>107</v>
-      </c>
-      <c r="F2" t="s">
-        <v>114</v>
-      </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A3" s="5" t="s">
@@ -3297,12 +3076,6 @@
       <c r="D3" t="s">
         <v>48</v>
       </c>
-      <c r="E3" t="s">
-        <v>108</v>
-      </c>
-      <c r="F3" t="s">
-        <v>110</v>
-      </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A4" s="5" t="s">
@@ -3413,22 +3186,18 @@
       </c>
     </row>
   </sheetData>
-  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G18"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:D18"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
-  <cols>
-    <col min="5" max="5" bestFit="true" customWidth="true" width="17.2578125" collapsed="true"/>
-    <col min="6" max="6" bestFit="true" customWidth="true" width="9.9453125" collapsed="true"/>
-  </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A1" s="5" t="s">
@@ -3443,12 +3212,6 @@
       <c r="D1" t="s">
         <v>92</v>
       </c>
-      <c r="E1" s="26" t="s">
-        <v>6</v>
-      </c>
-      <c r="F1" s="27" t="s">
-        <v>106</v>
-      </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A2" s="5" t="s">
@@ -3457,12 +3220,6 @@
       <c r="B2" s="8">
         <v>43362</v>
       </c>
-      <c r="E2" t="s">
-        <v>107</v>
-      </c>
-      <c r="F2" t="s">
-        <v>115</v>
-      </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A3" s="5" t="s">
@@ -3477,12 +3234,6 @@
       <c r="D3" t="s">
         <v>53</v>
       </c>
-      <c r="E3" t="s">
-        <v>108</v>
-      </c>
-      <c r="F3" t="s">
-        <v>110</v>
-      </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A4" s="5" t="s">
@@ -3585,22 +3336,18 @@
       </c>
     </row>
   </sheetData>
-  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G18"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:D18"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
-  <cols>
-    <col min="5" max="5" bestFit="true" customWidth="true" width="17.2578125" collapsed="true"/>
-    <col min="6" max="6" bestFit="true" customWidth="true" width="11.05859375" collapsed="false"/>
-  </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A1" s="5" t="s">
@@ -3615,12 +3362,6 @@
       <c r="D1" t="s">
         <v>92</v>
       </c>
-      <c r="E1" s="28" t="s">
-        <v>6</v>
-      </c>
-      <c r="F1" s="29" t="s">
-        <v>106</v>
-      </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A2" s="5" t="s">
@@ -3629,12 +3370,6 @@
       <c r="B2" s="8">
         <v>43362</v>
       </c>
-      <c r="E2" t="s">
-        <v>107</v>
-      </c>
-      <c r="F2" t="s">
-        <v>116</v>
-      </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A3" s="5" t="s">
@@ -3649,12 +3384,6 @@
       <c r="D3" t="s">
         <v>58</v>
       </c>
-      <c r="E3" t="s">
-        <v>108</v>
-      </c>
-      <c r="F3" t="s">
-        <v>110</v>
-      </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A4" s="5" t="s">
@@ -3765,14 +3494,14 @@
       </c>
     </row>
   </sheetData>
-  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C24"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:B24"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -3930,14 +3659,14 @@
       </c>
     </row>
   </sheetData>
-  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C24"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:B24"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -4095,7 +3824,7 @@
       </c>
     </row>
   </sheetData>
-  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>

</xml_diff>